<commit_message>
Agent step completed: Implement real-time updates using WebSockets
</commit_message>
<xml_diff>
--- a/static/whatsmyname_report_gorbash.xlsx
+++ b/static/whatsmyname_report_gorbash.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B118"/>
+  <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,24 +460,24 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bandlab</t>
+          <t>ask.fm</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
+          <t>https://ask.fm/gorbash</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ask.fm</t>
+          <t>Bandlab</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://ask.fm/gorbash</t>
+          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
         </is>
       </c>
     </row>
@@ -508,12 +508,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>cfx.re</t>
+          <t>chaturbate</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://forum.cfx.re/u/gorbash.json</t>
+          <t>https://chaturbate.com/gorbash/</t>
         </is>
       </c>
     </row>
@@ -532,24 +532,24 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>chaturbate</t>
+          <t>Chyoa</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://chaturbate.com/gorbash/</t>
+          <t>https://chyoa.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cda.pl</t>
+          <t>Chomikuj.pl</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.cda.pl/gorbash</t>
+          <t>https://chomikuj.pl/gorbash/</t>
         </is>
       </c>
     </row>
@@ -568,48 +568,48 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chomikuj.pl</t>
+          <t>cda.pl</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://chomikuj.pl/gorbash/</t>
+          <t>https://www.cda.pl/gorbash</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Codewars</t>
+          <t>cHEEZburger</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.codewars.com/users/gorbash</t>
+          <t>https://profile.cheezburger.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>cHEEZburger</t>
+          <t>cfx.re</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://profile.cheezburger.com/gorbash</t>
+          <t>https://forum.cfx.re/u/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chyoa</t>
+          <t>Codewars</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://chyoa.com/user/gorbash</t>
+          <t>https://www.codewars.com/users/gorbash</t>
         </is>
       </c>
     </row>
@@ -640,24 +640,24 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>diigo</t>
+          <t>Cults3D</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
+          <t>https://cults3d.com/en/users/gorbash/creations</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Disqus</t>
+          <t>diigo</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://disqus.com/by/gorbash/</t>
+          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
         </is>
       </c>
     </row>
@@ -676,48 +676,48 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Discogs</t>
+          <t>Disqus</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://api.discogs.com/users/gorbash</t>
+          <t>https://disqus.com/by/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DeviantArt</t>
+          <t>Discogs</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.deviantart.com/gorbash</t>
+          <t>https://api.discogs.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Cults3D</t>
+          <t>DockerHub</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://cults3d.com/en/users/gorbash/creations</t>
+          <t>https://hub.docker.com/v2/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DockerHub</t>
+          <t>DeviantArt</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://hub.docker.com/v2/users/gorbash/</t>
+          <t>https://www.deviantart.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -748,36 +748,36 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Demotywatory</t>
+          <t>Etsy</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://demotywatory.pl/user/gorbash</t>
+          <t>https://www.etsy.com/people/gorbash</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Etsy</t>
+          <t>Demotywatory</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/people/gorbash</t>
+          <t>https://demotywatory.pl/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Fabswingers</t>
+          <t>FatSecret</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.fabswingers.com/profile/gorbash</t>
+          <t>https://www.fatsecret.com/member/gorbash</t>
         </is>
       </c>
     </row>
@@ -808,12 +808,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>FatSecret</t>
+          <t>Fabswingers</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.fatsecret.com/member/gorbash</t>
+          <t>https://www.fabswingers.com/profile/gorbash</t>
         </is>
       </c>
     </row>
@@ -832,24 +832,24 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Filmweb</t>
+          <t>Foursquare</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.filmweb.pl/user/gorbash</t>
+          <t>https://foursquare.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Foursquare</t>
+          <t>Filmweb</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://foursquare.com/gorbash</t>
+          <t>https://www.filmweb.pl/user/gorbash</t>
         </is>
       </c>
     </row>
@@ -868,72 +868,72 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Flipboard</t>
+          <t>Geocaching</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://flipboard.com/@gorbash</t>
+          <t>https://www.geocaching.com/p/?u=gorbash</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Geocaching</t>
+          <t>Gravatar</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.geocaching.com/p/?u=gorbash</t>
+          <t>https://en.gravatar.com/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Gravatar</t>
+          <t>GitHub</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://en.gravatar.com/gorbash.json</t>
+          <t>https://github.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>GitHub</t>
+          <t>Flipboard</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://github.com/gorbash</t>
+          <t>https://flipboard.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>giters</t>
+          <t>GitLab</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://giters.com/gorbash</t>
+          <t>https://gitlab.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>GitLab</t>
+          <t>giters</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://gitlab.com/gorbash</t>
+          <t>https://giters.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -952,36 +952,36 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>HackerOne</t>
+          <t>HudsonRock</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://hackerone.com/gorbash</t>
+          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>HudsonRock</t>
+          <t>IFTTT</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
+          <t>https://ifttt.com/p/gorbash</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>IFTTT</t>
+          <t>HackerOne</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://ifttt.com/p/gorbash</t>
+          <t>https://hackerone.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -1012,96 +1012,96 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>issuu</t>
+          <t>inaturalist</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://issuu.com/gorbash</t>
+          <t>https://inaturalist.nz/people/gorbash</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>kaggle</t>
+          <t>issuu</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.kaggle.com/gorbash</t>
+          <t>https://issuu.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>inaturalist</t>
+          <t>Instagram2</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://inaturalist.nz/people/gorbash</t>
+          <t>https://dumpoir.com/v/gorbash</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Instagram2</t>
+          <t>kaggle</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://dumpoir.com/v/gorbash</t>
+          <t>https://www.kaggle.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Internet Archive User Search</t>
+          <t>Keybase</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
+          <t>https://keybase.io/gorbash</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Keybase</t>
+          <t>Jeuxvideo</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://keybase.io/gorbash</t>
+          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>InkBunny</t>
+          <t>Internet Archive User Search</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://inkbunny.net/gorbash</t>
+          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Jeuxvideo</t>
+          <t>Kongregate</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
+          <t>https://www.kongregate.com/accounts/gorbash</t>
         </is>
       </c>
     </row>
@@ -1120,12 +1120,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Kongregate</t>
+          <t>InkBunny</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.kongregate.com/accounts/gorbash</t>
+          <t>https://inkbunny.net/gorbash</t>
         </is>
       </c>
     </row>
@@ -1180,36 +1180,36 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Livejournal</t>
+          <t>MCUUID (Minecraft)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://gorbash.livejournal.com</t>
+          <t>https://playerdb.co/api/player/minecraft/gorbash</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Mastodon API</t>
+          <t>Livejournal</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
+          <t>https://gorbash.livejournal.com</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>MCUUID (Minecraft)</t>
+          <t>Mastodon API</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://playerdb.co/api/player/minecraft/gorbash</t>
+          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
         </is>
       </c>
     </row>
@@ -1228,24 +1228,24 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>MyAnimeList</t>
+          <t>MySpace</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://myanimelist.net/profile/gorbash</t>
+          <t>https://myspace.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MySpace</t>
+          <t>MyAnimeList</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://myspace.com/gorbash</t>
+          <t>https://myanimelist.net/profile/gorbash</t>
         </is>
       </c>
     </row>
@@ -1264,12 +1264,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>MCName (Minecraft)</t>
+          <t>palnet</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://mcname.info/en/search?q=gorbash</t>
+          <t>https://www.palnet.io/@gorbash/</t>
         </is>
       </c>
     </row>
@@ -1288,60 +1288,60 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>palnet</t>
+          <t>pikabu</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.palnet.io/@gorbash/</t>
+          <t>https://pikabu.ru/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>pikabu</t>
+          <t>Pinterest</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://pikabu.ru/@gorbash</t>
+          <t>https://www.pinterest.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Pinterest</t>
+          <t>Pokerstrategy</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.pinterest.com/gorbash/</t>
+          <t>http://www.pokerstrategy.net/user/gorbash/profile/</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Pokerstrategy</t>
+          <t>Periscope</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>http://www.pokerstrategy.net/user/gorbash/profile/</t>
+          <t>https://www.periscope.tv/gorbash</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Periscope</t>
+          <t>prv.pl</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.periscope.tv/gorbash</t>
+          <t>https://www.prv.pl/osoba/gorbash</t>
         </is>
       </c>
     </row>
@@ -1360,24 +1360,24 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>prv.pl</t>
+          <t>public</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.prv.pl/osoba/gorbash</t>
+          <t>https://public.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>public</t>
+          <t>Roblox</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://public.com/@gorbash</t>
+          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
         </is>
       </c>
     </row>
@@ -1396,36 +1396,36 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Roblox</t>
+          <t>MCName (Minecraft)</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
+          <t>https://mcname.info/en/search?q=gorbash</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>slideshare</t>
+          <t>RumbleUser</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://www.slideshare.net/gorbash</t>
+          <t>https://rumble.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>RumbleUser</t>
+          <t>slideshare</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://rumble.com/user/gorbash</t>
+          <t>https://www.slideshare.net/gorbash</t>
         </is>
       </c>
     </row>
@@ -1444,12 +1444,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>smule</t>
+          <t>SFD</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.smule.com/api/profile/?handle=gorbash</t>
+          <t>https://www.sfd.pl/profile/gorbash</t>
         </is>
       </c>
     </row>
@@ -1468,72 +1468,72 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>SFD</t>
+          <t>sofurry</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://www.sfd.pl/profile/gorbash</t>
+          <t>https://gorbash.sofurry.com</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>sofurry</t>
+          <t>SoundCloud</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://gorbash.sofurry.com</t>
+          <t>https://soundcloud.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>SoundCloud</t>
+          <t>Sourceforge</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://soundcloud.com/gorbash</t>
+          <t>https://sourceforge.net/u/gorbash/profile</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Sourceforge</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://sourceforge.net/u/gorbash/profile</t>
+          <t>https://open.spotify.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://open.spotify.com/user/gorbash</t>
+          <t>https://steamcommunity.com/id/gorbash</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>themeforest</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://steamcommunity.com/id/gorbash</t>
+          <t>https://themeforest.net/user/gorbash</t>
         </is>
       </c>
     </row>
@@ -1552,48 +1552,48 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>themeforest</t>
+          <t>Telegram</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://themeforest.net/user/gorbash</t>
+          <t>https://t.me/gorbash</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Telegram</t>
+          <t>TikTok</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://t.me/gorbash</t>
+          <t>https://www.tiktok.com/oembed?url=https://www.tiktok.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>TikTok</t>
+          <t>Trello</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/oembed?url=https://www.tiktok.com/@gorbash</t>
+          <t>https://trello.com/1/Members/gorbash?fields=activityBlocked%2CavatarUrl%2Cbio%2CbioData%2Cconfirmed%2CfullName%2CidEnterprise%2CidMemberReferrer%2Cinitials%2CmemberType%2CnonPublic%2Cproducts%2Curl%2Cusername</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Trello</t>
+          <t>Twitter archived profile</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://trello.com/1/Members/gorbash?fields=activityBlocked%2CavatarUrl%2Cbio%2CbioData%2Cconfirmed%2CfullName%2CidEnterprise%2CidMemberReferrer%2Cinitials%2CmemberType%2CnonPublic%2Cproducts%2Curl%2Cusername</t>
+          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -1624,36 +1624,36 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Twitch</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://nitter.privacydev.net/gorbash</t>
+          <t>https://twitchtracker.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Venmo</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://account.venmo.com/u/gorbash</t>
+          <t>https://nitter.privacydev.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>untappd</t>
+          <t>Venmo</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://untappd.com/user/gorbash/</t>
+          <t>https://account.venmo.com/u/gorbash</t>
         </is>
       </c>
     </row>
@@ -1672,24 +1672,24 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>wattpad</t>
+          <t>untappd</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
+          <t>https://untappd.com/user/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Twitch</t>
+          <t>wattpad</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://twitchtracker.com/gorbash</t>
+          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
         </is>
       </c>
     </row>
@@ -1720,36 +1720,36 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>VK</t>
+          <t>WordPress Support</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://vk.com/gorbash</t>
+          <t>https://wordpress.org/support/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>WordPress Support</t>
+          <t>VK</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://wordpress.org/support/users/gorbash/</t>
+          <t>https://vk.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>xHamster</t>
+          <t>YouTube User2</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://xhamster.com/users/gorbash</t>
+          <t>https://www.youtube.com/@gorbash</t>
         </is>
       </c>
     </row>
@@ -1768,12 +1768,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>YouTube User2</t>
+          <t>xHamster</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@gorbash</t>
+          <t>https://xhamster.com/users/gorbash</t>
         </is>
       </c>
     </row>
@@ -1822,18 +1822,6 @@
       <c r="B117" t="inlineStr">
         <is>
           <t>https://www.xnxx.com/mobile/profile/gorbash</t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>Twitter archived profile</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Agent step completed: Update search completion message in main.js
</commit_message>
<xml_diff>
--- a/static/whatsmyname_report_gorbash.xlsx
+++ b/static/whatsmyname_report_gorbash.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B117"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,24 +460,24 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ask.fm</t>
+          <t>Bandlab</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://ask.fm/gorbash</t>
+          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bandlab</t>
+          <t>ask.fm</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
+          <t>https://ask.fm/gorbash</t>
         </is>
       </c>
     </row>
@@ -496,60 +496,60 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Chess.com</t>
+          <t>cfx.re</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://api.chess.com/pub/player/gorbash</t>
+          <t>https://forum.cfx.re/u/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>chaturbate</t>
+          <t>chatango.com</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://chaturbate.com/gorbash/</t>
+          <t>https://gorbash.chatango.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>chatango.com</t>
+          <t>chaturbate</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://gorbash.chatango.com</t>
+          <t>https://chaturbate.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chyoa</t>
+          <t>Chess.com</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://chyoa.com/user/gorbash</t>
+          <t>https://api.chess.com/pub/player/gorbash</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chomikuj.pl</t>
+          <t>cda.pl</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://chomikuj.pl/gorbash/</t>
+          <t>https://www.cda.pl/gorbash</t>
         </is>
       </c>
     </row>
@@ -568,48 +568,48 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>cda.pl</t>
+          <t>Chomikuj.pl</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.cda.pl/gorbash</t>
+          <t>https://chomikuj.pl/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>cHEEZburger</t>
+          <t>Codewars</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://profile.cheezburger.com/gorbash</t>
+          <t>https://www.codewars.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>cfx.re</t>
+          <t>cHEEZburger</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://forum.cfx.re/u/gorbash.json</t>
+          <t>https://profile.cheezburger.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Codewars</t>
+          <t>Chyoa</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://www.codewars.com/users/gorbash</t>
+          <t>https://chyoa.com/user/gorbash</t>
         </is>
       </c>
     </row>
@@ -640,48 +640,48 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Cults3D</t>
+          <t>diigo</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://cults3d.com/en/users/gorbash/creations</t>
+          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>diigo</t>
+          <t>Disqus</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
+          <t>https://disqus.com/by/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Dating.ru</t>
+          <t>DeviantArt</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://dating.ru/gorbash/</t>
+          <t>https://www.deviantart.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Disqus</t>
+          <t>Dating.ru</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://disqus.com/by/gorbash/</t>
+          <t>https://dating.ru/gorbash/</t>
         </is>
       </c>
     </row>
@@ -712,12 +712,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DeviantArt</t>
+          <t>Cults3D</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.deviantart.com/gorbash</t>
+          <t>https://cults3d.com/en/users/gorbash/creations</t>
         </is>
       </c>
     </row>
@@ -772,24 +772,24 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>FatSecret</t>
+          <t>Fark</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.fatsecret.com/member/gorbash</t>
+          <t>https://www.fark.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Fark</t>
+          <t>Fabswingers</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.fark.com/users/gorbash</t>
+          <t>https://www.fabswingers.com/profile/gorbash</t>
         </is>
       </c>
     </row>
@@ -808,12 +808,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Fabswingers</t>
+          <t>FatSecret</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.fabswingers.com/profile/gorbash</t>
+          <t>https://www.fatsecret.com/member/gorbash</t>
         </is>
       </c>
     </row>
@@ -856,36 +856,36 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>FurAffinity</t>
+          <t>Flipboard</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.furaffinity.net/user/gorbash</t>
+          <t>https://flipboard.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Geocaching</t>
+          <t>FurAffinity</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.geocaching.com/p/?u=gorbash</t>
+          <t>https://www.furaffinity.net/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Gravatar</t>
+          <t>Geocaching</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://en.gravatar.com/gorbash.json</t>
+          <t>https://www.geocaching.com/p/?u=gorbash</t>
         </is>
       </c>
     </row>
@@ -904,12 +904,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Flipboard</t>
+          <t>Gravatar</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://flipboard.com/@gorbash</t>
+          <t>https://en.gravatar.com/gorbash.json</t>
         </is>
       </c>
     </row>
@@ -964,120 +964,120 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>IFTTT</t>
+          <t>HackerOne</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://ifttt.com/p/gorbash</t>
+          <t>https://hackerone.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>HackerOne</t>
+          <t>FriendFinder-X</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://hackerone.com/gorbash</t>
+          <t>https://www.friendfinder-x.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>hugging_face</t>
+          <t>IFTTT</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://huggingface.co/gorbash</t>
+          <t>https://ifttt.com/p/gorbash</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>imgur</t>
+          <t>hugging_face</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://api.imgur.com/account/v1/accounts/gorbash?client_id=546c25a59c58ad7&amp;include=trophies%2Cmedallions</t>
+          <t>https://huggingface.co/gorbash</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>inaturalist</t>
+          <t>imgur</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://inaturalist.nz/people/gorbash</t>
+          <t>https://api.imgur.com/account/v1/accounts/gorbash?client_id=546c25a59c58ad7&amp;include=trophies%2Cmedallions</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>issuu</t>
+          <t>inaturalist</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://issuu.com/gorbash</t>
+          <t>https://inaturalist.nz/people/gorbash</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Instagram2</t>
+          <t>InkBunny</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://dumpoir.com/v/gorbash</t>
+          <t>https://inkbunny.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>kaggle</t>
+          <t>Instagram2</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.kaggle.com/gorbash</t>
+          <t>https://dumpoir.com/v/gorbash</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Keybase</t>
+          <t>kaggle</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://keybase.io/gorbash</t>
+          <t>https://www.kaggle.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Jeuxvideo</t>
+          <t>issuu</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
+          <t>https://issuu.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -1096,48 +1096,48 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Kongregate</t>
+          <t>Keybase</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.kongregate.com/accounts/gorbash</t>
+          <t>https://keybase.io/gorbash</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Linktree</t>
+          <t>Kongregate</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://linktr.ee/gorbash</t>
+          <t>https://www.kongregate.com/accounts/gorbash</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>InkBunny</t>
+          <t>Linktree</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://inkbunny.net/gorbash</t>
+          <t>https://linktr.ee/gorbash</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>FriendFinder-X</t>
+          <t>Jeuxvideo</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.friendfinder-x.com/profile/gorbash</t>
+          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
         </is>
       </c>
     </row>
@@ -1180,36 +1180,36 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>MCUUID (Minecraft)</t>
+          <t>Mastodon API</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://playerdb.co/api/player/minecraft/gorbash</t>
+          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Livejournal</t>
+          <t>MCUUID (Minecraft)</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://gorbash.livejournal.com</t>
+          <t>https://playerdb.co/api/player/minecraft/gorbash</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Mastodon API</t>
+          <t>Livejournal</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
+          <t>https://gorbash.livejournal.com</t>
         </is>
       </c>
     </row>
@@ -1264,12 +1264,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>palnet</t>
+          <t>MCName (Minecraft)</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.palnet.io/@gorbash/</t>
+          <t>https://mcname.info/en/search?q=gorbash</t>
         </is>
       </c>
     </row>
@@ -1336,12 +1336,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>prv.pl</t>
+          <t>palnet</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.prv.pl/osoba/gorbash</t>
+          <t>https://www.palnet.io/@gorbash/</t>
         </is>
       </c>
     </row>
@@ -1360,48 +1360,48 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>public</t>
+          <t>prv.pl</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://public.com/@gorbash</t>
+          <t>https://www.prv.pl/osoba/gorbash</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Roblox</t>
+          <t>public</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
+          <t>https://public.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>rsi</t>
+          <t>Roblox</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://robertsspaceindustries.com/citizens/gorbash</t>
+          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>MCName (Minecraft)</t>
+          <t>rsi</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://mcname.info/en/search?q=gorbash</t>
+          <t>https://robertsspaceindustries.com/citizens/gorbash</t>
         </is>
       </c>
     </row>
@@ -1468,36 +1468,36 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>sofurry</t>
+          <t>SoundCloud</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://gorbash.sofurry.com</t>
+          <t>https://soundcloud.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>SoundCloud</t>
+          <t>Sourceforge</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://soundcloud.com/gorbash</t>
+          <t>https://sourceforge.net/u/gorbash/profile</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Sourceforge</t>
+          <t>sofurry</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://sourceforge.net/u/gorbash/profile</t>
+          <t>https://gorbash.sofurry.com</t>
         </is>
       </c>
     </row>
@@ -1528,36 +1528,36 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>themeforest</t>
+          <t>tabletoptournament</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://themeforest.net/user/gorbash</t>
+          <t>https://www.tabletoptournaments.net/eu/player/gorbash</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>tabletoptournament</t>
+          <t>Telegram</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://www.tabletoptournaments.net/eu/player/gorbash</t>
+          <t>https://t.me/gorbash</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Telegram</t>
+          <t>themeforest</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://t.me/gorbash</t>
+          <t>https://themeforest.net/user/gorbash</t>
         </is>
       </c>
     </row>
@@ -1588,238 +1588,226 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Twitter archived profile</t>
+          <t>trakt</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash</t>
+          <t>https://trakt.tv/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>trakt</t>
+          <t>tumblr</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://trakt.tv/users/gorbash</t>
+          <t>https://gorbash.tumblr.com</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>tumblr</t>
+          <t>Twitch</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://gorbash.tumblr.com</t>
+          <t>https://twitchtracker.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Twitch</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://twitchtracker.com/gorbash</t>
+          <t>https://nitter.privacydev.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Venmo</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://nitter.privacydev.net/gorbash</t>
+          <t>https://account.venmo.com/u/gorbash</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Venmo</t>
+          <t>Vimeo</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://account.venmo.com/u/gorbash</t>
+          <t>https://vimeo.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Vimeo</t>
+          <t>untappd</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://vimeo.com/gorbash</t>
+          <t>https://untappd.com/user/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>untappd</t>
+          <t>wattpad</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://untappd.com/user/gorbash/</t>
+          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>wattpad</t>
+          <t>Wikidot</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
+          <t>http://www.wikidot.com/user:info/gorbash</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Wikidot</t>
+          <t>Xbox Gamertag</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>http://www.wikidot.com/user:info/gorbash</t>
+          <t>https://www.xboxgamertag.com/search/gorbash</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Xbox Gamertag</t>
+          <t>WordPress Support</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://www.xboxgamertag.com/search/gorbash</t>
+          <t>https://wordpress.org/support/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>WordPress Support</t>
+          <t>VK</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://wordpress.org/support/users/gorbash/</t>
+          <t>https://vk.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>VK</t>
+          <t>xHamster</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://vk.com/gorbash</t>
+          <t>https://xhamster.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>YouTube User2</t>
+          <t>YouTube User</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@gorbash</t>
+          <t>https://www.youtube.com/user/gorbash/about</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>YouTube User</t>
+          <t>YouTube User2</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/user/gorbash/about</t>
+          <t>https://www.youtube.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>xHamster</t>
+          <t>XVIDEOS-profiles</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://xhamster.com/users/gorbash</t>
+          <t>https://www.xvideos.com/profiles/gorbash</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>XVIDEOS-profiles</t>
+          <t>XVIDEOS-models</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://www.xvideos.com/profiles/gorbash</t>
+          <t>https://www.xvideos.com/models/gorbash</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>XVIDEOS-models</t>
+          <t>Zbiornik</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://www.xvideos.com/models/gorbash</t>
+          <t>https://mini.zbiornik.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Zbiornik</t>
+          <t>XNXX</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
-        <is>
-          <t>https://mini.zbiornik.com/gorbash</t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>XNXX</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
         <is>
           <t>https://www.xnxx.com/mobile/profile/gorbash</t>
         </is>

</xml_diff>

<commit_message>
Agent step completed: Implement clear command for the terminal
</commit_message>
<xml_diff>
--- a/static/whatsmyname_report_gorbash.xlsx
+++ b/static/whatsmyname_report_gorbash.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,24 +460,24 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Bandlab</t>
+          <t>ask.fm</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
+          <t>https://ask.fm/gorbash</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ask.fm</t>
+          <t>Bandlab</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://ask.fm/gorbash</t>
+          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
         </is>
       </c>
     </row>
@@ -496,84 +496,84 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cfx.re</t>
+          <t>chaturbate</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://forum.cfx.re/u/gorbash.json</t>
+          <t>https://chaturbate.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>chatango.com</t>
+          <t>Chess.com</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://gorbash.chatango.com</t>
+          <t>https://api.chess.com/pub/player/gorbash</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>chaturbate</t>
+          <t>chatango.com</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://chaturbate.com/gorbash/</t>
+          <t>https://gorbash.chatango.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chess.com</t>
+          <t>cfx.re</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://api.chess.com/pub/player/gorbash</t>
+          <t>https://forum.cfx.re/u/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cda.pl</t>
+          <t>Chomikuj.pl</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.cda.pl/gorbash</t>
+          <t>https://chomikuj.pl/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Code Project</t>
+          <t>cda.pl</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.codeproject.com/Members/gorbash</t>
+          <t>https://www.cda.pl/gorbash</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chomikuj.pl</t>
+          <t>Code Project</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://chomikuj.pl/gorbash/</t>
+          <t>https://www.codeproject.com/Members/gorbash</t>
         </is>
       </c>
     </row>
@@ -640,120 +640,120 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>diigo</t>
+          <t>DeviantArt</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
+          <t>https://www.deviantart.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Disqus</t>
+          <t>diigo</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://disqus.com/by/gorbash/</t>
+          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>DeviantArt</t>
+          <t>Discogs</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.deviantart.com/gorbash</t>
+          <t>https://api.discogs.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dating.ru</t>
+          <t>Disqus</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://dating.ru/gorbash/</t>
+          <t>https://disqus.com/by/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Discogs</t>
+          <t>DockerHub</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://api.discogs.com/users/gorbash</t>
+          <t>https://hub.docker.com/v2/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>DockerHub</t>
+          <t>Cults3D</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://hub.docker.com/v2/users/gorbash/</t>
+          <t>https://cults3d.com/en/users/gorbash/creations</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cults3D</t>
+          <t>datezone</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://cults3d.com/en/users/gorbash/creations</t>
+          <t>https://www.datezone.com/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>datezone</t>
+          <t>Duolingo</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.datezone.com/users/gorbash/</t>
+          <t>https://www.duolingo.com/2017-06-30/users?username=gorbash&amp;_=1628308619574</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Duolingo</t>
+          <t>Etsy</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.duolingo.com/2017-06-30/users?username=gorbash&amp;_=1628308619574</t>
+          <t>https://www.etsy.com/people/gorbash</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Etsy</t>
+          <t>Fark</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/people/gorbash</t>
+          <t>https://www.fark.com/users/gorbash</t>
         </is>
       </c>
     </row>
@@ -772,408 +772,408 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Fark</t>
+          <t>Fabswingers</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.fark.com/users/gorbash</t>
+          <t>https://www.fabswingers.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Fabswingers</t>
+          <t>fansly</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.fabswingers.com/profile/gorbash</t>
+          <t>https://apiv2.fansly.com/api/v1/account?usernames=gorbash</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>eBay</t>
+          <t>FatSecret</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/usr/gorbash</t>
+          <t>https://www.fatsecret.com/member/gorbash</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>FatSecret</t>
+          <t>Filmweb</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.fatsecret.com/member/gorbash</t>
+          <t>https://www.filmweb.pl/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>fansly</t>
+          <t>Foursquare</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://apiv2.fansly.com/api/v1/account?usernames=gorbash</t>
+          <t>https://foursquare.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Foursquare</t>
+          <t>Flipboard</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://foursquare.com/gorbash</t>
+          <t>https://flipboard.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Filmweb</t>
+          <t>FurAffinity</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.filmweb.pl/user/gorbash</t>
+          <t>https://www.furaffinity.net/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Flipboard</t>
+          <t>Geocaching</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://flipboard.com/@gorbash</t>
+          <t>https://www.geocaching.com/p/?u=gorbash</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>FurAffinity</t>
+          <t>giters</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.furaffinity.net/user/gorbash</t>
+          <t>https://giters.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Geocaching</t>
+          <t>GitHub</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.geocaching.com/p/?u=gorbash</t>
+          <t>https://github.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GitHub</t>
+          <t>Gravatar</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://github.com/gorbash</t>
+          <t>https://en.gravatar.com/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Gravatar</t>
+          <t>GitLab</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://en.gravatar.com/gorbash.json</t>
+          <t>https://gitlab.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>GitLab</t>
+          <t>Hacker News</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://gitlab.com/gorbash</t>
+          <t>https://news.ycombinator.com/user?id=gorbash</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>giters</t>
+          <t>HudsonRock</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://giters.com/gorbash</t>
+          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Hacker News</t>
+          <t>HackerOne</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://news.ycombinator.com/user?id=gorbash</t>
+          <t>https://hackerone.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>HudsonRock</t>
+          <t>IFTTT</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
+          <t>https://ifttt.com/p/gorbash</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>HackerOne</t>
+          <t>hugging_face</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://hackerone.com/gorbash</t>
+          <t>https://huggingface.co/gorbash</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>FriendFinder-X</t>
+          <t>imgur</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.friendfinder-x.com/profile/gorbash</t>
+          <t>https://api.imgur.com/account/v1/accounts/gorbash?client_id=546c25a59c58ad7&amp;include=trophies%2Cmedallions</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>IFTTT</t>
+          <t>InkBunny</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://ifttt.com/p/gorbash</t>
+          <t>https://inkbunny.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>hugging_face</t>
+          <t>inaturalist</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://huggingface.co/gorbash</t>
+          <t>https://inaturalist.nz/people/gorbash</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>imgur</t>
+          <t>issuu</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://api.imgur.com/account/v1/accounts/gorbash?client_id=546c25a59c58ad7&amp;include=trophies%2Cmedallions</t>
+          <t>https://issuu.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>inaturalist</t>
+          <t>Internet Archive User Search</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://inaturalist.nz/people/gorbash</t>
+          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>InkBunny</t>
+          <t>Instagram2</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://inkbunny.net/gorbash</t>
+          <t>https://dumpoir.com/v/gorbash</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Instagram2</t>
+          <t>kaggle</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://dumpoir.com/v/gorbash</t>
+          <t>https://www.kaggle.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>kaggle</t>
+          <t>Jeuxvideo</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.kaggle.com/gorbash</t>
+          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>issuu</t>
+          <t>Keybase</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://issuu.com/gorbash</t>
+          <t>https://keybase.io/gorbash</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Internet Archive User Search</t>
+          <t>Linktree</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
+          <t>https://linktr.ee/gorbash</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Keybase</t>
+          <t>Kongregate</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://keybase.io/gorbash</t>
+          <t>https://www.kongregate.com/accounts/gorbash</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Kongregate</t>
+          <t>LibraryThing</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.kongregate.com/accounts/gorbash</t>
+          <t>https://www.librarything.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Linktree</t>
+          <t>lichess</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://linktr.ee/gorbash</t>
+          <t>https://lichess.org/@/gorbash</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Jeuxvideo</t>
+          <t>waytohey</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
+          <t>https://waytohey.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>lichess</t>
+          <t>FriendFinder-X</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://lichess.org/@/gorbash</t>
+          <t>https://www.friendfinder-x.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>LibraryThing</t>
+          <t>Livejournal</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://www.librarything.com/profile/gorbash</t>
+          <t>https://gorbash.livejournal.com</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>waytohey</t>
+          <t>MCUUID (Minecraft)</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://waytohey.com/gorbash</t>
+          <t>https://playerdb.co/api/player/minecraft/gorbash</t>
         </is>
       </c>
     </row>
@@ -1192,468 +1192,468 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>MCUUID (Minecraft)</t>
+          <t>Mod DB</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://playerdb.co/api/player/minecraft/gorbash</t>
+          <t>https://www.moddb.com/members/gorbash</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Livejournal</t>
+          <t>MyAnimeList</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://gorbash.livejournal.com</t>
+          <t>https://myanimelist.net/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Mod DB</t>
+          <t>MySpace</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://www.moddb.com/members/gorbash</t>
+          <t>https://myspace.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>MySpace</t>
+          <t>OpenStreetMap</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://myspace.com/gorbash</t>
+          <t>https://www.openstreetmap.org/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MyAnimeList</t>
+          <t>MCName (Minecraft)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://myanimelist.net/profile/gorbash</t>
+          <t>https://mcname.info/en/search?q=gorbash</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>OpenStreetMap</t>
+          <t>palnet</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.openstreetmap.org/user/gorbash</t>
+          <t>https://www.palnet.io/@gorbash/</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>MCName (Minecraft)</t>
+          <t>Playstation Network</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://mcname.info/en/search?q=gorbash</t>
+          <t>https://psnprofiles.com/xhr/search/users?q=gorbash</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Playstation Network</t>
+          <t>pikabu</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://psnprofiles.com/xhr/search/users?q=gorbash</t>
+          <t>https://pikabu.ru/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>pikabu</t>
+          <t>Pinterest</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://pikabu.ru/@gorbash</t>
+          <t>https://www.pinterest.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Pinterest</t>
+          <t>Pokerstrategy</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://www.pinterest.com/gorbash/</t>
+          <t>http://www.pokerstrategy.net/user/gorbash/profile/</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Pokerstrategy</t>
+          <t>Periscope</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>http://www.pokerstrategy.net/user/gorbash/profile/</t>
+          <t>https://www.periscope.tv/gorbash</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Periscope</t>
+          <t>prv.pl</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.periscope.tv/gorbash</t>
+          <t>https://www.prv.pl/osoba/gorbash</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>palnet</t>
+          <t>Pornhub Users</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.palnet.io/@gorbash/</t>
+          <t>https://www.pornhub.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Pornhub Users</t>
+          <t>public</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.pornhub.com/users/gorbash</t>
+          <t>https://public.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>prv.pl</t>
+          <t>Roblox</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.prv.pl/osoba/gorbash</t>
+          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>public</t>
+          <t>rsi</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://public.com/@gorbash</t>
+          <t>https://robertsspaceindustries.com/citizens/gorbash</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Roblox</t>
+          <t>RumbleUser</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
+          <t>https://rumble.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>rsi</t>
+          <t>slideshare</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://robertsspaceindustries.com/citizens/gorbash</t>
+          <t>https://www.slideshare.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>RumbleUser</t>
+          <t>sentimente</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://rumble.com/user/gorbash</t>
+          <t>https://www.sentimente.com/amp/gorbash.html</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>slideshare</t>
+          <t>Snapchat Stories</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://www.slideshare.net/gorbash</t>
+          <t>https://story.snapchat.com/s/gorbash</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>sentimente</t>
+          <t>SFD</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.sentimente.com/amp/gorbash.html</t>
+          <t>https://www.sfd.pl/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>SFD</t>
+          <t>sofurry</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.sfd.pl/profile/gorbash</t>
+          <t>https://gorbash.sofurry.com</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Snapchat Stories</t>
+          <t>SoundCloud</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://story.snapchat.com/s/gorbash</t>
+          <t>https://soundcloud.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>SoundCloud</t>
+          <t>Sourceforge</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://soundcloud.com/gorbash</t>
+          <t>https://sourceforge.net/u/gorbash/profile</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Sourceforge</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://sourceforge.net/u/gorbash/profile</t>
+          <t>https://open.spotify.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>sofurry</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://gorbash.sofurry.com</t>
+          <t>https://steamcommunity.com/id/gorbash</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>themeforest</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://open.spotify.com/user/gorbash</t>
+          <t>https://themeforest.net/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>TikTok</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://steamcommunity.com/id/gorbash</t>
+          <t>https://www.tiktok.com/oembed?url=https://www.tiktok.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>tabletoptournament</t>
+          <t>Telegram</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://www.tabletoptournaments.net/eu/player/gorbash</t>
+          <t>https://t.me/gorbash</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Telegram</t>
+          <t>Twitter archived tweets</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://t.me/gorbash</t>
+          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash/status/*</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>themeforest</t>
+          <t>Trello</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://themeforest.net/user/gorbash</t>
+          <t>https://trello.com/1/Members/gorbash?fields=activityBlocked%2CavatarUrl%2Cbio%2CbioData%2Cconfirmed%2CfullName%2CidEnterprise%2CidMemberReferrer%2Cinitials%2CmemberType%2CnonPublic%2Cproducts%2Curl%2Cusername</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>TikTok</t>
+          <t>trakt</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/oembed?url=https://www.tiktok.com/@gorbash</t>
+          <t>https://trakt.tv/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Trello</t>
+          <t>tumblr</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://trello.com/1/Members/gorbash?fields=activityBlocked%2CavatarUrl%2Cbio%2CbioData%2Cconfirmed%2CfullName%2CidEnterprise%2CidMemberReferrer%2Cinitials%2CmemberType%2CnonPublic%2Cproducts%2Curl%2Cusername</t>
+          <t>https://gorbash.tumblr.com</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>trakt</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://trakt.tv/users/gorbash</t>
+          <t>https://nitter.privacydev.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>tumblr</t>
+          <t>Twitch</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://gorbash.tumblr.com</t>
+          <t>https://twitchtracker.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Twitch</t>
+          <t>Vimeo</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://twitchtracker.com/gorbash</t>
+          <t>https://vimeo.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Venmo</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://nitter.privacydev.net/gorbash</t>
+          <t>https://account.venmo.com/u/gorbash</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Venmo</t>
+          <t>wattpad</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://account.venmo.com/u/gorbash</t>
+          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Vimeo</t>
+          <t>Wikidot</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://vimeo.com/gorbash</t>
+          <t>http://www.wikidot.com/user:info/gorbash</t>
         </is>
       </c>
     </row>
@@ -1672,142 +1672,118 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>wattpad</t>
+          <t>Xbox Gamertag</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
+          <t>https://www.xboxgamertag.com/search/gorbash</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Wikidot</t>
+          <t>WordPress Support</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>http://www.wikidot.com/user:info/gorbash</t>
+          <t>https://wordpress.org/support/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Xbox Gamertag</t>
+          <t>VK</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://www.xboxgamertag.com/search/gorbash</t>
+          <t>https://vk.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>WordPress Support</t>
+          <t>xHamster</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://wordpress.org/support/users/gorbash/</t>
+          <t>https://xhamster.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>VK</t>
+          <t>YouTube User</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://vk.com/gorbash</t>
+          <t>https://www.youtube.com/user/gorbash/about</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>xHamster</t>
+          <t>YouTube User2</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://xhamster.com/users/gorbash</t>
+          <t>https://www.youtube.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>YouTube User</t>
+          <t>XVIDEOS-profiles</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/user/gorbash/about</t>
+          <t>https://www.xvideos.com/profiles/gorbash</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>YouTube User2</t>
+          <t>XVIDEOS-models</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@gorbash</t>
+          <t>https://www.xvideos.com/models/gorbash</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>XVIDEOS-profiles</t>
+          <t>Zbiornik</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://www.xvideos.com/profiles/gorbash</t>
+          <t>https://mini.zbiornik.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>XVIDEOS-models</t>
+          <t>XNXX</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
-        <is>
-          <t>https://www.xvideos.com/models/gorbash</t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>Zbiornik</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>https://mini.zbiornik.com/gorbash</t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>XNXX</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
         <is>
           <t>https://www.xnxx.com/mobile/profile/gorbash</t>
         </is>

</xml_diff>

<commit_message>
Agent step completed: Add creator information under the WhatsMyName Web logo
</commit_message>
<xml_diff>
--- a/static/whatsmyname_report_gorbash.xlsx
+++ b/static/whatsmyname_report_gorbash.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B114"/>
+  <dimension ref="A1:B116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,228 +472,228 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bandlab</t>
+          <t>BodyBuilding.com</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
+          <t>http://api.bodybuilding.com/api-proxy/bbc/get?slug=gorbash</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BodyBuilding.com</t>
+          <t>Chess.com</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://api.bodybuilding.com/api-proxy/bbc/get?slug=gorbash</t>
+          <t>https://api.chess.com/pub/player/gorbash</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>chaturbate</t>
+          <t>cfx.re</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://chaturbate.com/gorbash/</t>
+          <t>https://forum.cfx.re/u/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Chess.com</t>
+          <t>chatango.com</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://api.chess.com/pub/player/gorbash</t>
+          <t>https://gorbash.chatango.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>chatango.com</t>
+          <t>chaturbate</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://gorbash.chatango.com</t>
+          <t>https://chaturbate.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>cfx.re</t>
+          <t>cda.pl</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://forum.cfx.re/u/gorbash.json</t>
+          <t>https://www.cda.pl/gorbash</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chomikuj.pl</t>
+          <t>Code Project</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://chomikuj.pl/gorbash/</t>
+          <t>https://www.codeproject.com/Members/gorbash</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>cda.pl</t>
+          <t>Codewars</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.cda.pl/gorbash</t>
+          <t>https://www.codewars.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Code Project</t>
+          <t>cHEEZburger</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.codeproject.com/Members/gorbash</t>
+          <t>https://profile.cheezburger.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Codewars</t>
+          <t>Chyoa</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://www.codewars.com/users/gorbash</t>
+          <t>https://chyoa.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>cHEEZburger</t>
+          <t>Chomikuj.pl</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://profile.cheezburger.com/gorbash</t>
+          <t>https://chomikuj.pl/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chyoa</t>
+          <t>crowdin</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://chyoa.com/user/gorbash</t>
+          <t>https://crowdin.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>crowdin</t>
+          <t>Mastodon-Defcon</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://crowdin.com/profile/gorbash</t>
+          <t>https://defcon.social/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Mastodon-Defcon</t>
+          <t>diigo</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://defcon.social/@gorbash</t>
+          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DeviantArt</t>
+          <t>Discogs</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://www.deviantart.com/gorbash</t>
+          <t>https://api.discogs.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>diigo</t>
+          <t>Dating.ru</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
+          <t>https://dating.ru/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Discogs</t>
+          <t>Disqus</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://api.discogs.com/users/gorbash</t>
+          <t>https://disqus.com/by/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Disqus</t>
+          <t>DockerHub</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://disqus.com/by/gorbash/</t>
+          <t>https://hub.docker.com/v2/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DockerHub</t>
+          <t>DeviantArt</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://hub.docker.com/v2/users/gorbash/</t>
+          <t>https://www.deviantart.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -736,168 +736,168 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Etsy</t>
+          <t>Demotywatory</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/people/gorbash</t>
+          <t>https://demotywatory.pl/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Fark</t>
+          <t>eBay</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.fark.com/users/gorbash</t>
+          <t>https://www.ebay.com/usr/gorbash</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Demotywatory</t>
+          <t>Etsy</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://demotywatory.pl/user/gorbash</t>
+          <t>https://www.etsy.com/people/gorbash</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Fabswingers</t>
+          <t>Fark</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.fabswingers.com/profile/gorbash</t>
+          <t>https://www.fark.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>fansly</t>
+          <t>FatSecret</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://apiv2.fansly.com/api/v1/account?usernames=gorbash</t>
+          <t>https://www.fatsecret.com/member/gorbash</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>FatSecret</t>
+          <t>fansly</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.fatsecret.com/member/gorbash</t>
+          <t>https://apiv2.fansly.com/api/v1/account?usernames=gorbash</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Filmweb</t>
+          <t>Fabswingers</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.filmweb.pl/user/gorbash</t>
+          <t>https://www.fabswingers.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Foursquare</t>
+          <t>Flipboard</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://foursquare.com/gorbash</t>
+          <t>https://flipboard.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Flipboard</t>
+          <t>FurAffinity</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://flipboard.com/@gorbash</t>
+          <t>https://www.furaffinity.net/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>FurAffinity</t>
+          <t>Foursquare</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.furaffinity.net/user/gorbash</t>
+          <t>https://foursquare.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Geocaching</t>
+          <t>Filmweb</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.geocaching.com/p/?u=gorbash</t>
+          <t>https://www.filmweb.pl/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>giters</t>
+          <t>Geocaching</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://giters.com/gorbash</t>
+          <t>https://www.geocaching.com/p/?u=gorbash</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>GitHub</t>
+          <t>Gravatar</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://github.com/gorbash</t>
+          <t>https://en.gravatar.com/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Gravatar</t>
+          <t>GitHub</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://en.gravatar.com/gorbash.json</t>
+          <t>https://github.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -916,84 +916,84 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Hacker News</t>
+          <t>HackerOne</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://news.ycombinator.com/user?id=gorbash</t>
+          <t>https://hackerone.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>HudsonRock</t>
+          <t>Hacker News</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
+          <t>https://news.ycombinator.com/user?id=gorbash</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>HackerOne</t>
+          <t>giters</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://hackerone.com/gorbash</t>
+          <t>https://giters.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>IFTTT</t>
+          <t>FriendFinder-X</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://ifttt.com/p/gorbash</t>
+          <t>https://www.friendfinder-x.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>hugging_face</t>
+          <t>IFTTT</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://huggingface.co/gorbash</t>
+          <t>https://ifttt.com/p/gorbash</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>imgur</t>
+          <t>hugging_face</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://api.imgur.com/account/v1/accounts/gorbash?client_id=546c25a59c58ad7&amp;include=trophies%2Cmedallions</t>
+          <t>https://huggingface.co/gorbash</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>InkBunny</t>
+          <t>imgur</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://inkbunny.net/gorbash</t>
+          <t>https://api.imgur.com/account/v1/accounts/gorbash?client_id=546c25a59c58ad7&amp;include=trophies%2Cmedallions</t>
         </is>
       </c>
     </row>
@@ -1012,60 +1012,60 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>issuu</t>
+          <t>InkBunny</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://issuu.com/gorbash</t>
+          <t>https://inkbunny.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Internet Archive User Search</t>
+          <t>issuu</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
+          <t>https://issuu.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Instagram2</t>
+          <t>HudsonRock</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://dumpoir.com/v/gorbash</t>
+          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>kaggle</t>
+          <t>Instagram2</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.kaggle.com/gorbash</t>
+          <t>https://dumpoir.com/v/gorbash</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Jeuxvideo</t>
+          <t>kaggle</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
+          <t>https://www.kaggle.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -1084,84 +1084,84 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Linktree</t>
+          <t>Internet Archive User Search</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://linktr.ee/gorbash</t>
+          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Kongregate</t>
+          <t>Jeuxvideo</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.kongregate.com/accounts/gorbash</t>
+          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>LibraryThing</t>
+          <t>Kongregate</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.librarything.com/profile/gorbash</t>
+          <t>https://www.kongregate.com/accounts/gorbash</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>lichess</t>
+          <t>Linktree</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://lichess.org/@/gorbash</t>
+          <t>https://linktr.ee/gorbash</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>waytohey</t>
+          <t>LibraryThing</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://waytohey.com/gorbash</t>
+          <t>https://www.librarything.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>FriendFinder-X</t>
+          <t>Mastodon API</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://www.friendfinder-x.com/profile/gorbash</t>
+          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Livejournal</t>
+          <t>waytohey</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://gorbash.livejournal.com</t>
+          <t>https://waytohey.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -1180,12 +1180,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Mastodon API</t>
+          <t>Livejournal</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
+          <t>https://gorbash.livejournal.com</t>
         </is>
       </c>
     </row>
@@ -1240,60 +1240,60 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MCName (Minecraft)</t>
+          <t>Playstation Network</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://mcname.info/en/search?q=gorbash</t>
+          <t>https://psnprofiles.com/xhr/search/users?q=gorbash</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>palnet</t>
+          <t>pikabu</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.palnet.io/@gorbash/</t>
+          <t>https://pikabu.ru/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Playstation Network</t>
+          <t>Pinterest</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://psnprofiles.com/xhr/search/users?q=gorbash</t>
+          <t>https://www.pinterest.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>pikabu</t>
+          <t>MCName (Minecraft)</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://pikabu.ru/@gorbash</t>
+          <t>https://mcname.info/en/search?q=gorbash</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Pinterest</t>
+          <t>Periscope</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.pinterest.com/gorbash/</t>
+          <t>https://www.periscope.tv/gorbash</t>
         </is>
       </c>
     </row>
@@ -1312,12 +1312,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Periscope</t>
+          <t>palnet</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.periscope.tv/gorbash</t>
+          <t>https://www.palnet.io/@gorbash/</t>
         </is>
       </c>
     </row>
@@ -1336,24 +1336,24 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Pornhub Users</t>
+          <t>public</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.pornhub.com/users/gorbash</t>
+          <t>https://public.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>public</t>
+          <t>Pornhub Users</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://public.com/@gorbash</t>
+          <t>https://www.pornhub.com/users/gorbash</t>
         </is>
       </c>
     </row>
@@ -1384,36 +1384,36 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>RumbleUser</t>
+          <t>sentimente</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://rumble.com/user/gorbash</t>
+          <t>https://www.sentimente.com/amp/gorbash.html</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>slideshare</t>
+          <t>SFD</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.slideshare.net/gorbash</t>
+          <t>https://www.sfd.pl/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>sentimente</t>
+          <t>RumbleUser</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://www.sentimente.com/amp/gorbash.html</t>
+          <t>https://rumble.com/user/gorbash</t>
         </is>
       </c>
     </row>
@@ -1432,120 +1432,120 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>SFD</t>
+          <t>sofurry</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.sfd.pl/profile/gorbash</t>
+          <t>https://gorbash.sofurry.com</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>sofurry</t>
+          <t>slideshare</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://gorbash.sofurry.com</t>
+          <t>https://www.slideshare.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>SoundCloud</t>
+          <t>Sourceforge</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://soundcloud.com/gorbash</t>
+          <t>https://sourceforge.net/u/gorbash/profile</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Sourceforge</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://sourceforge.net/u/gorbash/profile</t>
+          <t>https://steamcommunity.com/id/gorbash</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>SoundCloud</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://open.spotify.com/user/gorbash</t>
+          <t>https://soundcloud.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://steamcommunity.com/id/gorbash</t>
+          <t>https://open.spotify.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>themeforest</t>
+          <t>tabletoptournament</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://themeforest.net/user/gorbash</t>
+          <t>https://www.tabletoptournaments.net/eu/player/gorbash</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>TikTok</t>
+          <t>Telegram</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/oembed?url=https://www.tiktok.com/@gorbash</t>
+          <t>https://t.me/gorbash</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Telegram</t>
+          <t>themeforest</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://t.me/gorbash</t>
+          <t>https://themeforest.net/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Twitter archived tweets</t>
+          <t>TikTok</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash/status/*</t>
+          <t>https://www.tiktok.com/oembed?url=https://www.tiktok.com/@gorbash</t>
         </is>
       </c>
     </row>
@@ -1588,156 +1588,156 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Twitter archived profile</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://nitter.privacydev.net/gorbash</t>
+          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Twitch</t>
+          <t>Twitter archived tweets</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://twitchtracker.com/gorbash</t>
+          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash/status/*</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Vimeo</t>
+          <t>Venmo</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://vimeo.com/gorbash</t>
+          <t>https://account.venmo.com/u/gorbash</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Venmo</t>
+          <t>untappd</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://account.venmo.com/u/gorbash</t>
+          <t>https://untappd.com/user/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>wattpad</t>
+          <t>Vimeo</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
+          <t>https://vimeo.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Wikidot</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>http://www.wikidot.com/user:info/gorbash</t>
+          <t>https://nitter.privacydev.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>untappd</t>
+          <t>Twitch</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://untappd.com/user/gorbash/</t>
+          <t>https://twitchtracker.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Xbox Gamertag</t>
+          <t>wattpad</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.xboxgamertag.com/search/gorbash</t>
+          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>WordPress Support</t>
+          <t>Wikidot</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://wordpress.org/support/users/gorbash/</t>
+          <t>http://www.wikidot.com/user:info/gorbash</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>VK</t>
+          <t>WordPress Support</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://vk.com/gorbash</t>
+          <t>https://wordpress.org/support/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>xHamster</t>
+          <t>VK</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://xhamster.com/users/gorbash</t>
+          <t>https://vk.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>YouTube User</t>
+          <t>xHamster</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/user/gorbash/about</t>
+          <t>https://xhamster.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>YouTube User2</t>
+          <t>YouTube User</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@gorbash</t>
+          <t>https://www.youtube.com/user/gorbash/about</t>
         </is>
       </c>
     </row>
@@ -1756,36 +1756,60 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>XVIDEOS-models</t>
+          <t>YouTube User2</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.xvideos.com/models/gorbash</t>
+          <t>https://www.youtube.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Zbiornik</t>
+          <t>XVIDEOS-models</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://mini.zbiornik.com/gorbash</t>
+          <t>https://www.xvideos.com/models/gorbash</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
+          <t>Zbiornik</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>https://mini.zbiornik.com/gorbash</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
           <t>XNXX</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
+      <c r="B115" t="inlineStr">
         <is>
           <t>https://www.xnxx.com/mobile/profile/gorbash</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Xbox Gamertag</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>https://www.xboxgamertag.com/search/gorbash</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Checkpoint before revert - Replace blinking emoji with clickable green eye icon
</commit_message>
<xml_diff>
--- a/static/whatsmyname_report_gorbash.xlsx
+++ b/static/whatsmyname_report_gorbash.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,72 +448,72 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Audiojungle</t>
+          <t>Bandlab</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://audiojungle.net/user/gorbash</t>
+          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ask.fm</t>
+          <t>Audiojungle</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://ask.fm/gorbash</t>
+          <t>https://audiojungle.net/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BodyBuilding.com</t>
+          <t>ask.fm</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://api.bodybuilding.com/api-proxy/bbc/get?slug=gorbash</t>
+          <t>https://ask.fm/gorbash</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Chess.com</t>
+          <t>BodyBuilding.com</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://api.chess.com/pub/player/gorbash</t>
+          <t>http://api.bodybuilding.com/api-proxy/bbc/get?slug=gorbash</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cfx.re</t>
+          <t>Chess.com</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://forum.cfx.re/u/gorbash.json</t>
+          <t>https://api.chess.com/pub/player/gorbash</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>chatango.com</t>
+          <t>cfx.re</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://gorbash.chatango.com</t>
+          <t>https://forum.cfx.re/u/gorbash.json</t>
         </is>
       </c>
     </row>
@@ -532,168 +532,168 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>cda.pl</t>
+          <t>chatango.com</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.cda.pl/gorbash</t>
+          <t>https://gorbash.chatango.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Code Project</t>
+          <t>cda.pl</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.codeproject.com/Members/gorbash</t>
+          <t>https://www.cda.pl/gorbash</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Codewars</t>
+          <t>Code Project</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.codewars.com/users/gorbash</t>
+          <t>https://www.codeproject.com/Members/gorbash</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>cHEEZburger</t>
+          <t>Codewars</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://profile.cheezburger.com/gorbash</t>
+          <t>https://www.codewars.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Chyoa</t>
+          <t>Chomikuj.pl</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://chyoa.com/user/gorbash</t>
+          <t>https://chomikuj.pl/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chomikuj.pl</t>
+          <t>Chyoa</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://chomikuj.pl/gorbash/</t>
+          <t>https://chyoa.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>crowdin</t>
+          <t>cHEEZburger</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://crowdin.com/profile/gorbash</t>
+          <t>https://profile.cheezburger.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Mastodon-Defcon</t>
+          <t>crowdin</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://defcon.social/@gorbash</t>
+          <t>https://crowdin.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>diigo</t>
+          <t>Mastodon-Defcon</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
+          <t>https://defcon.social/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Discogs</t>
+          <t>diigo</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://api.discogs.com/users/gorbash</t>
+          <t>https://www.diigo.com/interact_api/load_profile_info?name=gorbash</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dating.ru</t>
+          <t>Disqus</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://dating.ru/gorbash/</t>
+          <t>https://disqus.com/by/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Disqus</t>
+          <t>Discogs</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://disqus.com/by/gorbash/</t>
+          <t>https://api.discogs.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>DockerHub</t>
+          <t>Dating.ru</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://hub.docker.com/v2/users/gorbash/</t>
+          <t>https://dating.ru/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DeviantArt</t>
+          <t>DockerHub</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.deviantart.com/gorbash</t>
+          <t>https://hub.docker.com/v2/users/gorbash/</t>
         </is>
       </c>
     </row>
@@ -724,48 +724,48 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Duolingo</t>
+          <t>DeviantArt</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.duolingo.com/2017-06-30/users?username=gorbash&amp;_=1628308619574</t>
+          <t>https://www.deviantart.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Demotywatory</t>
+          <t>Duolingo</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://demotywatory.pl/user/gorbash</t>
+          <t>https://www.duolingo.com/2017-06-30/users?username=gorbash&amp;_=1628308619574</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>eBay</t>
+          <t>Etsy</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/usr/gorbash</t>
+          <t>https://www.etsy.com/people/gorbash</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Etsy</t>
+          <t>eBay</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/people/gorbash</t>
+          <t>https://www.ebay.com/usr/gorbash</t>
         </is>
       </c>
     </row>
@@ -796,60 +796,60 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>fansly</t>
+          <t>Fabswingers</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://apiv2.fansly.com/api/v1/account?usernames=gorbash</t>
+          <t>https://www.fabswingers.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Fabswingers</t>
+          <t>Demotywatory</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.fabswingers.com/profile/gorbash</t>
+          <t>https://demotywatory.pl/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Flipboard</t>
+          <t>fansly</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://flipboard.com/@gorbash</t>
+          <t>https://apiv2.fansly.com/api/v1/account?usernames=gorbash</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>FurAffinity</t>
+          <t>Foursquare</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.furaffinity.net/user/gorbash</t>
+          <t>https://foursquare.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Foursquare</t>
+          <t>Flipboard</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://foursquare.com/gorbash</t>
+          <t>https://flipboard.com/@gorbash</t>
         </is>
       </c>
     </row>
@@ -868,12 +868,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Geocaching</t>
+          <t>FurAffinity</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.geocaching.com/p/?u=gorbash</t>
+          <t>https://www.furaffinity.net/user/gorbash</t>
         </is>
       </c>
     </row>
@@ -892,72 +892,72 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GitHub</t>
+          <t>Geocaching</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://github.com/gorbash</t>
+          <t>https://www.geocaching.com/p/?u=gorbash</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>GitLab</t>
+          <t>GitHub</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://gitlab.com/gorbash</t>
+          <t>https://github.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>HackerOne</t>
+          <t>GitLab</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://hackerone.com/gorbash</t>
+          <t>https://gitlab.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Hacker News</t>
+          <t>HackerOne</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://news.ycombinator.com/user?id=gorbash</t>
+          <t>https://hackerone.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>giters</t>
+          <t>Hacker News</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://giters.com/gorbash</t>
+          <t>https://news.ycombinator.com/user?id=gorbash</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>FriendFinder-X</t>
+          <t>HudsonRock</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.friendfinder-x.com/profile/gorbash</t>
+          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>HudsonRock</t>
+          <t>kaggle</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
+          <t>https://www.kaggle.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -1060,108 +1060,108 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>kaggle</t>
+          <t>Internet Archive User Search</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.kaggle.com/gorbash</t>
+          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Keybase</t>
+          <t>Jeuxvideo</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://keybase.io/gorbash</t>
+          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Internet Archive User Search</t>
+          <t>Keybase</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
+          <t>https://keybase.io/gorbash</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Jeuxvideo</t>
+          <t>Kongregate</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
+          <t>https://www.kongregate.com/accounts/gorbash</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Kongregate</t>
+          <t>Linktree</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.kongregate.com/accounts/gorbash</t>
+          <t>https://linktr.ee/gorbash</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Linktree</t>
+          <t>LibraryThing</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://linktr.ee/gorbash</t>
+          <t>https://www.librarything.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>LibraryThing</t>
+          <t>FriendFinder-X</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.librarything.com/profile/gorbash</t>
+          <t>https://www.friendfinder-x.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Mastodon API</t>
+          <t>waytohey</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
+          <t>https://waytohey.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>waytohey</t>
+          <t>Livejournal</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://waytohey.com/gorbash</t>
+          <t>https://gorbash.livejournal.com</t>
         </is>
       </c>
     </row>
@@ -1180,12 +1180,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Livejournal</t>
+          <t>Mastodon API</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://gorbash.livejournal.com</t>
+          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
         </is>
       </c>
     </row>
@@ -1240,216 +1240,216 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Playstation Network</t>
+          <t>MCName (Minecraft)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://psnprofiles.com/xhr/search/users?q=gorbash</t>
+          <t>https://mcname.info/en/search?q=gorbash</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>pikabu</t>
+          <t>Playstation Network</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://pikabu.ru/@gorbash</t>
+          <t>https://psnprofiles.com/xhr/search/users?q=gorbash</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Pinterest</t>
+          <t>pikabu</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.pinterest.com/gorbash/</t>
+          <t>https://pikabu.ru/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>MCName (Minecraft)</t>
+          <t>Pokerstrategy</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://mcname.info/en/search?q=gorbash</t>
+          <t>http://www.pokerstrategy.net/user/gorbash/profile/</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Periscope</t>
+          <t>palnet</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.periscope.tv/gorbash</t>
+          <t>https://www.palnet.io/@gorbash/</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Pokerstrategy</t>
+          <t>Pinterest</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>http://www.pokerstrategy.net/user/gorbash/profile/</t>
+          <t>https://www.pinterest.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>palnet</t>
+          <t>Periscope</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.palnet.io/@gorbash/</t>
+          <t>https://www.periscope.tv/gorbash</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>prv.pl</t>
+          <t>public</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.prv.pl/osoba/gorbash</t>
+          <t>https://public.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>public</t>
+          <t>Pornhub Users</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://public.com/@gorbash</t>
+          <t>https://www.pornhub.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Pornhub Users</t>
+          <t>prv.pl</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.pornhub.com/users/gorbash</t>
+          <t>https://www.prv.pl/osoba/gorbash</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Roblox</t>
+          <t>rsi</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
+          <t>https://robertsspaceindustries.com/citizens/gorbash</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>rsi</t>
+          <t>Roblox</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://robertsspaceindustries.com/citizens/gorbash</t>
+          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>sentimente</t>
+          <t>RumbleUser</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.sentimente.com/amp/gorbash.html</t>
+          <t>https://rumble.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>SFD</t>
+          <t>slideshare</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.sfd.pl/profile/gorbash</t>
+          <t>https://www.slideshare.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>RumbleUser</t>
+          <t>sentimente</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://rumble.com/user/gorbash</t>
+          <t>https://www.sentimente.com/amp/gorbash.html</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Snapchat Stories</t>
+          <t>SFD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://story.snapchat.com/s/gorbash</t>
+          <t>https://www.sfd.pl/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>sofurry</t>
+          <t>smule</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://gorbash.sofurry.com</t>
+          <t>https://www.smule.com/api/profile/?handle=gorbash</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>slideshare</t>
+          <t>Snapchat Stories</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.slideshare.net/gorbash</t>
+          <t>https://story.snapchat.com/s/gorbash</t>
         </is>
       </c>
     </row>
@@ -1504,24 +1504,24 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>tabletoptournament</t>
+          <t>sofurry</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://www.tabletoptournaments.net/eu/player/gorbash</t>
+          <t>https://gorbash.sofurry.com</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Telegram</t>
+          <t>tabletoptournament</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://t.me/gorbash</t>
+          <t>https://www.tabletoptournaments.net/eu/player/gorbash</t>
         </is>
       </c>
     </row>
@@ -1552,156 +1552,156 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Trello</t>
+          <t>Telegram</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://trello.com/1/Members/gorbash?fields=activityBlocked%2CavatarUrl%2Cbio%2CbioData%2Cconfirmed%2CfullName%2CidEnterprise%2CidMemberReferrer%2Cinitials%2CmemberType%2CnonPublic%2Cproducts%2Curl%2Cusername</t>
+          <t>https://t.me/gorbash</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>trakt</t>
+          <t>Trello</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://trakt.tv/users/gorbash</t>
+          <t>https://trello.com/1/Members/gorbash?fields=activityBlocked%2CavatarUrl%2Cbio%2CbioData%2Cconfirmed%2CfullName%2CidEnterprise%2CidMemberReferrer%2Cinitials%2CmemberType%2CnonPublic%2Cproducts%2Curl%2Cusername</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>tumblr</t>
+          <t>trakt</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://gorbash.tumblr.com</t>
+          <t>https://trakt.tv/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Twitter archived profile</t>
+          <t>tumblr</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash</t>
+          <t>https://gorbash.tumblr.com</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Twitter archived tweets</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash/status/*</t>
+          <t>https://nitter.privacydev.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Venmo</t>
+          <t>Twitter archived profile</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://account.venmo.com/u/gorbash</t>
+          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>untappd</t>
+          <t>Twitter archived tweets</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://untappd.com/user/gorbash/</t>
+          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash/status/*</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Vimeo</t>
+          <t>Venmo</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://vimeo.com/gorbash</t>
+          <t>https://account.venmo.com/u/gorbash</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Vimeo</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://nitter.privacydev.net/gorbash</t>
+          <t>https://vimeo.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Twitch</t>
+          <t>untappd</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://twitchtracker.com/gorbash</t>
+          <t>https://untappd.com/user/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>wattpad</t>
+          <t>Twitch</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
+          <t>https://twitchtracker.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Wikidot</t>
+          <t>wattpad</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>http://www.wikidot.com/user:info/gorbash</t>
+          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>WordPress Support</t>
+          <t>Wikidot</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://wordpress.org/support/users/gorbash/</t>
+          <t>http://www.wikidot.com/user:info/gorbash</t>
         </is>
       </c>
     </row>
@@ -1720,94 +1720,106 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>xHamster</t>
+          <t>WordPress Support</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://xhamster.com/users/gorbash</t>
+          <t>https://wordpress.org/support/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>YouTube User</t>
+          <t>YouTube User2</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/user/gorbash/about</t>
+          <t>https://www.youtube.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>XVIDEOS-profiles</t>
+          <t>YouTube User</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://www.xvideos.com/profiles/gorbash</t>
+          <t>https://www.youtube.com/user/gorbash/about</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>YouTube User2</t>
+          <t>xHamster</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@gorbash</t>
+          <t>https://xhamster.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>XVIDEOS-models</t>
+          <t>XVIDEOS-profiles</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://www.xvideos.com/models/gorbash</t>
+          <t>https://www.xvideos.com/profiles/gorbash</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Zbiornik</t>
+          <t>XVIDEOS-models</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://mini.zbiornik.com/gorbash</t>
+          <t>https://www.xvideos.com/models/gorbash</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>XNXX</t>
+          <t>Zbiornik</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://www.xnxx.com/mobile/profile/gorbash</t>
+          <t>https://mini.zbiornik.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
+          <t>XNXX</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>https://www.xnxx.com/mobile/profile/gorbash</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
           <t>Xbox Gamertag</t>
         </is>
       </c>
-      <c r="B116" t="inlineStr">
+      <c r="B117" t="inlineStr">
         <is>
           <t>https://www.xboxgamertag.com/search/gorbash</t>
         </is>

</xml_diff>

<commit_message>
Agent step completed: Add cloud icon and implement color scheme toggle
</commit_message>
<xml_diff>
--- a/static/whatsmyname_report_gorbash.xlsx
+++ b/static/whatsmyname_report_gorbash.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,24 +448,24 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Audiojungle</t>
+          <t>Bandlab</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://audiojungle.net/user/gorbash</t>
+          <t>https://www.bandlab.com/api/v1.3/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ask.fm</t>
+          <t>Audiojungle</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://ask.fm/gorbash</t>
+          <t>https://audiojungle.net/user/gorbash</t>
         </is>
       </c>
     </row>
@@ -496,36 +496,36 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cfx.re</t>
+          <t>chaturbate</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://forum.cfx.re/u/gorbash.json</t>
+          <t>https://chaturbate.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>chatango.com</t>
+          <t>cfx.re</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://gorbash.chatango.com</t>
+          <t>https://forum.cfx.re/u/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>chaturbate</t>
+          <t>chatango.com</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://chaturbate.com/gorbash/</t>
+          <t>https://gorbash.chatango.com</t>
         </is>
       </c>
     </row>
@@ -544,60 +544,60 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Code Project</t>
+          <t>Chyoa</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.codeproject.com/Members/gorbash</t>
+          <t>https://chyoa.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Codewars</t>
+          <t>Chomikuj.pl</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.codewars.com/users/gorbash</t>
+          <t>https://chomikuj.pl/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>cHEEZburger</t>
+          <t>Code Project</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://profile.cheezburger.com/gorbash</t>
+          <t>https://www.codeproject.com/Members/gorbash</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Chyoa</t>
+          <t>Codewars</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://chyoa.com/user/gorbash</t>
+          <t>https://www.codewars.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chomikuj.pl</t>
+          <t>cHEEZburger</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://chomikuj.pl/gorbash/</t>
+          <t>https://profile.cheezburger.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -640,36 +640,36 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Discogs</t>
+          <t>Disqus</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://api.discogs.com/users/gorbash</t>
+          <t>https://disqus.com/by/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dating.ru</t>
+          <t>DeviantArt</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://dating.ru/gorbash/</t>
+          <t>https://www.deviantart.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Disqus</t>
+          <t>Discogs</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://disqus.com/by/gorbash/</t>
+          <t>https://api.discogs.com/users/gorbash</t>
         </is>
       </c>
     </row>
@@ -688,84 +688,84 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>DeviantArt</t>
+          <t>Dating.ru</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.deviantart.com/gorbash</t>
+          <t>https://dating.ru/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Cults3D</t>
+          <t>datezone</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://cults3d.com/en/users/gorbash/creations</t>
+          <t>https://www.datezone.com/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>datezone</t>
+          <t>Duolingo</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.datezone.com/users/gorbash/</t>
+          <t>https://www.duolingo.com/2017-06-30/users?username=gorbash&amp;_=1628308619574</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Duolingo</t>
+          <t>Cults3D</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.duolingo.com/2017-06-30/users?username=gorbash&amp;_=1628308619574</t>
+          <t>https://cults3d.com/en/users/gorbash/creations</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Demotywatory</t>
+          <t>Etsy</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://demotywatory.pl/user/gorbash</t>
+          <t>https://www.etsy.com/people/gorbash</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>eBay</t>
+          <t>Demotywatory</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.ebay.com/usr/gorbash</t>
+          <t>https://demotywatory.pl/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Etsy</t>
+          <t>eBay</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.etsy.com/people/gorbash</t>
+          <t>https://www.ebay.com/usr/gorbash</t>
         </is>
       </c>
     </row>
@@ -796,108 +796,108 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>fansly</t>
+          <t>Fabswingers</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://apiv2.fansly.com/api/v1/account?usernames=gorbash</t>
+          <t>https://www.fabswingers.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Fabswingers</t>
+          <t>Filmweb</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.fabswingers.com/profile/gorbash</t>
+          <t>https://www.filmweb.pl/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Flipboard</t>
+          <t>fansly</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://flipboard.com/@gorbash</t>
+          <t>https://apiv2.fansly.com/api/v1/account?usernames=gorbash</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>FurAffinity</t>
+          <t>Foursquare</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.furaffinity.net/user/gorbash</t>
+          <t>https://foursquare.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Foursquare</t>
+          <t>FurAffinity</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://foursquare.com/gorbash</t>
+          <t>https://www.furaffinity.net/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Filmweb</t>
+          <t>Geocaching</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.filmweb.pl/user/gorbash</t>
+          <t>https://www.geocaching.com/p/?u=gorbash</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Geocaching</t>
+          <t>Gravatar</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.geocaching.com/p/?u=gorbash</t>
+          <t>https://en.gravatar.com/gorbash.json</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Gravatar</t>
+          <t>GitHub</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://en.gravatar.com/gorbash.json</t>
+          <t>https://github.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>GitHub</t>
+          <t>giters</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://github.com/gorbash</t>
+          <t>https://giters.com/gorbash</t>
         </is>
       </c>
     </row>
@@ -940,36 +940,36 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>giters</t>
+          <t>HudsonRock</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://giters.com/gorbash</t>
+          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>FriendFinder-X</t>
+          <t>IFTTT</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.friendfinder-x.com/profile/gorbash</t>
+          <t>https://ifttt.com/p/gorbash</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>IFTTT</t>
+          <t>FriendFinder-X</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://ifttt.com/p/gorbash</t>
+          <t>https://www.friendfinder-x.com/profile/gorbash</t>
         </is>
       </c>
     </row>
@@ -1036,156 +1036,156 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>HudsonRock</t>
+          <t>Instagram2</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://cavalier.hudsonrock.com/api/json/v2/osint-tools/search-by-username?username=gorbash</t>
+          <t>https://dumpoir.com/v/gorbash</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Instagram2</t>
+          <t>kaggle</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://dumpoir.com/v/gorbash</t>
+          <t>https://www.kaggle.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>kaggle</t>
+          <t>Jeuxvideo</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.kaggle.com/gorbash</t>
+          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Keybase</t>
+          <t>Internet Archive User Search</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://keybase.io/gorbash</t>
+          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Internet Archive User Search</t>
+          <t>Keybase</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://archive.org/advancedsearch.php?q=gorbash&amp;output=json</t>
+          <t>https://keybase.io/gorbash</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Jeuxvideo</t>
+          <t>Kongregate</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.jeuxvideo.com/profil/gorbash?mode=infos</t>
+          <t>https://www.kongregate.com/accounts/gorbash</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Kongregate</t>
+          <t>Linktree</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.kongregate.com/accounts/gorbash</t>
+          <t>https://linktr.ee/gorbash</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Linktree</t>
+          <t>ask.fm</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://linktr.ee/gorbash</t>
+          <t>https://ask.fm/gorbash</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>LibraryThing</t>
+          <t>waytohey</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.librarything.com/profile/gorbash</t>
+          <t>https://waytohey.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Mastodon API</t>
+          <t>LibraryThing</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
+          <t>https://www.librarything.com/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>waytohey</t>
+          <t>Livejournal</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://waytohey.com/gorbash</t>
+          <t>https://gorbash.livejournal.com</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>MCUUID (Minecraft)</t>
+          <t>Mastodon API</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://playerdb.co/api/player/minecraft/gorbash</t>
+          <t>https://mastodon.social/api/v2/search?q=gorbash&amp;limit=1&amp;type=accounts</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Livejournal</t>
+          <t>MCUUID (Minecraft)</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://gorbash.livejournal.com</t>
+          <t>https://playerdb.co/api/player/minecraft/gorbash</t>
         </is>
       </c>
     </row>
@@ -1204,24 +1204,24 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>MyAnimeList</t>
+          <t>MySpace</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://myanimelist.net/profile/gorbash</t>
+          <t>https://myspace.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MySpace</t>
+          <t>MyAnimeList</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://myspace.com/gorbash</t>
+          <t>https://myanimelist.net/profile/gorbash</t>
         </is>
       </c>
     </row>
@@ -1240,48 +1240,48 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Playstation Network</t>
+          <t>MCName (Minecraft)</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://psnprofiles.com/xhr/search/users?q=gorbash</t>
+          <t>https://mcname.info/en/search?q=gorbash</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>pikabu</t>
+          <t>palnet</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://pikabu.ru/@gorbash</t>
+          <t>https://www.palnet.io/@gorbash/</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Pinterest</t>
+          <t>Pokerstrategy</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.pinterest.com/gorbash/</t>
+          <t>http://www.pokerstrategy.net/user/gorbash/profile/</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>MCName (Minecraft)</t>
+          <t>Playstation Network</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://mcname.info/en/search?q=gorbash</t>
+          <t>https://psnprofiles.com/xhr/search/users?q=gorbash</t>
         </is>
       </c>
     </row>
@@ -1300,48 +1300,48 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Pokerstrategy</t>
+          <t>pikabu</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>http://www.pokerstrategy.net/user/gorbash/profile/</t>
+          <t>https://pikabu.ru/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>palnet</t>
+          <t>Pinterest</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.palnet.io/@gorbash/</t>
+          <t>https://www.pinterest.com/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>prv.pl</t>
+          <t>Flipboard</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.prv.pl/osoba/gorbash</t>
+          <t>https://flipboard.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>public</t>
+          <t>prv.pl</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://public.com/@gorbash</t>
+          <t>https://www.prv.pl/osoba/gorbash</t>
         </is>
       </c>
     </row>
@@ -1360,48 +1360,48 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Roblox</t>
+          <t>public</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
+          <t>https://public.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>rsi</t>
+          <t>Roblox</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://robertsspaceindustries.com/citizens/gorbash</t>
+          <t>https://auth.roblox.com/v1/usernames/validate?username=gorbash&amp;birthday=2019-12-31T23:00:00.000Z</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>sentimente</t>
+          <t>rsi</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.sentimente.com/amp/gorbash.html</t>
+          <t>https://robertsspaceindustries.com/citizens/gorbash</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>SFD</t>
+          <t>sentimente</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.sfd.pl/profile/gorbash</t>
+          <t>https://www.sentimente.com/amp/gorbash.html</t>
         </is>
       </c>
     </row>
@@ -1420,132 +1420,132 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Snapchat Stories</t>
+          <t>SFD</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://story.snapchat.com/s/gorbash</t>
+          <t>https://www.sfd.pl/profile/gorbash</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>sofurry</t>
+          <t>slideshare</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://gorbash.sofurry.com</t>
+          <t>https://www.slideshare.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>slideshare</t>
+          <t>SoundCloud</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.slideshare.net/gorbash</t>
+          <t>https://soundcloud.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Sourceforge</t>
+          <t>smule</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://sourceforge.net/u/gorbash/profile</t>
+          <t>https://www.smule.com/api/profile/?handle=gorbash</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Steam</t>
+          <t>Sourceforge</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://steamcommunity.com/id/gorbash</t>
+          <t>https://sourceforge.net/u/gorbash/profile</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>SoundCloud</t>
+          <t>sofurry</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://soundcloud.com/gorbash</t>
+          <t>https://gorbash.sofurry.com</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Spotify</t>
+          <t>Snapchat Stories</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://open.spotify.com/user/gorbash</t>
+          <t>https://story.snapchat.com/s/gorbash</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>tabletoptournament</t>
+          <t>Spotify</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://www.tabletoptournaments.net/eu/player/gorbash</t>
+          <t>https://open.spotify.com/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Telegram</t>
+          <t>Steam</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://t.me/gorbash</t>
+          <t>https://steamcommunity.com/id/gorbash</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>themeforest</t>
+          <t>Telegram</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://themeforest.net/user/gorbash</t>
+          <t>https://t.me/gorbash</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>TikTok</t>
+          <t>tabletoptournament</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://www.tiktok.com/oembed?url=https://www.tiktok.com/@gorbash</t>
+          <t>https://www.tabletoptournaments.net/eu/player/gorbash</t>
         </is>
       </c>
     </row>
@@ -1564,144 +1564,144 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>trakt</t>
+          <t>themeforest</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://trakt.tv/users/gorbash</t>
+          <t>https://themeforest.net/user/gorbash</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>tumblr</t>
+          <t>TikTok</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://gorbash.tumblr.com</t>
+          <t>https://www.tiktok.com/oembed?url=https://www.tiktok.com/@gorbash</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Twitter archived profile</t>
+          <t>trakt</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash</t>
+          <t>https://trakt.tv/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Twitter archived tweets</t>
+          <t>tumblr</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash/status/*</t>
+          <t>https://gorbash.tumblr.com</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Venmo</t>
+          <t>Twitter</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://account.venmo.com/u/gorbash</t>
+          <t>https://nitter.privacydev.net/gorbash</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>untappd</t>
+          <t>Twitch</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://untappd.com/user/gorbash/</t>
+          <t>https://twitchtracker.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Vimeo</t>
+          <t>Twitter archived tweets</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://vimeo.com/gorbash</t>
+          <t>http://archive.org/wayback/available?url=https://twitter.com/gorbash/status/*</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Twitter</t>
+          <t>Vimeo</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://nitter.privacydev.net/gorbash</t>
+          <t>https://vimeo.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Twitch</t>
+          <t>Venmo</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://twitchtracker.com/gorbash</t>
+          <t>https://account.venmo.com/u/gorbash</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>wattpad</t>
+          <t>untappd</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
+          <t>https://untappd.com/user/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Wikidot</t>
+          <t>wattpad</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>http://www.wikidot.com/user:info/gorbash</t>
+          <t>https://www.wattpad.com/api/v3/users/gorbash?fields=username%2Cname%2Cdescription%2Cavatar%2CbackgroundUrl%2CcreateDate%2Clocation%2Cfollowing%2CfollowingRequest%2CnumFollowing%2Cfollower%2CfollowerRequest%2CnumFollowers%2CnumLists%2CnumStoriesPublished%2CvotesReceived%2Cfacebook%2Ctwitter%2Cwebsite%2Csmashwords%2Chighlight_colour%2Chtml_enabled%2Cverified%2Cambassador%2Cwattpad_squad%2Cis_staff%2Cprograms(wattpad_stars)%2CisPrivate%2CisMuted%2CexternalId%2Cnotes</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>WordPress Support</t>
+          <t>Wikidot</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://wordpress.org/support/users/gorbash/</t>
+          <t>http://www.wikidot.com/user:info/gorbash</t>
         </is>
       </c>
     </row>
@@ -1720,96 +1720,108 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>xHamster</t>
+          <t>Xbox Gamertag</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://xhamster.com/users/gorbash</t>
+          <t>https://www.xboxgamertag.com/search/gorbash</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>YouTube User</t>
+          <t>WordPress Support</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/user/gorbash/about</t>
+          <t>https://wordpress.org/support/users/gorbash/</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>XVIDEOS-profiles</t>
+          <t>xHamster</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://www.xvideos.com/profiles/gorbash</t>
+          <t>https://xhamster.com/users/gorbash</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>YouTube User2</t>
+          <t>Zbiornik</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.youtube.com/@gorbash</t>
+          <t>https://mini.zbiornik.com/gorbash</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>XVIDEOS-models</t>
+          <t>XVIDEOS-profiles</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://www.xvideos.com/models/gorbash</t>
+          <t>https://www.xvideos.com/profiles/gorbash</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Zbiornik</t>
+          <t>XVIDEOS-models</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://mini.zbiornik.com/gorbash</t>
+          <t>https://www.xvideos.com/models/gorbash</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>XNXX</t>
+          <t>YouTube User</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://www.xnxx.com/mobile/profile/gorbash</t>
+          <t>https://www.youtube.com/user/gorbash/about</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Xbox Gamertag</t>
+          <t>YouTube User2</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://www.xboxgamertag.com/search/gorbash</t>
+          <t>https://www.youtube.com/@gorbash</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>XNXX</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>https://www.xnxx.com/mobile/profile/gorbash</t>
         </is>
       </c>
     </row>

</xml_diff>